<commit_message>
Update Código Efecto Hall
</commit_message>
<xml_diff>
--- a/4. Efecto Hall/Code/Datos_VL_n.xlsx
+++ b/4. Efecto Hall/Code/Datos_VL_n.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\Intermedio\4. Efecto Hall\CompleteData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F85B8FC-0E0A-4FEA-B385-8F7A5D99683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33E722F-A3FC-4582-85E4-81035A6FE0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2436" yWindow="2508" windowWidth="11160" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -66,22 +66,22 @@
     <t>B_rounded (mT)</t>
   </si>
   <si>
-    <t>VL_-20mA (mV)</t>
-  </si>
-  <si>
-    <t>VL_-10mA (mV)</t>
-  </si>
-  <si>
-    <t>VL_10mA (mV)</t>
-  </si>
-  <si>
-    <t>VL_20mA (mV)</t>
-  </si>
-  <si>
-    <t>VL_err (mV)</t>
-  </si>
-  <si>
     <t>B_err_rounded (mT)</t>
+  </si>
+  <si>
+    <t>VL_-20mA (V)</t>
+  </si>
+  <si>
+    <t>VL_-10mA (V)</t>
+  </si>
+  <si>
+    <t>VL_10mA (V)</t>
+  </si>
+  <si>
+    <t>VL_20mA (V)</t>
+  </si>
+  <si>
+    <t>VL_err (V)</t>
   </si>
 </sst>
 </file>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,22 +545,22 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -596,7 +596,7 @@
         <v>0.74399999999999999</v>
       </c>
       <c r="J2">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -632,7 +632,7 @@
         <v>0.74099999999999999</v>
       </c>
       <c r="J3">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -668,7 +668,7 @@
         <v>0.73799999999999999</v>
       </c>
       <c r="J4">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -704,7 +704,7 @@
         <v>0.73599999999999999</v>
       </c>
       <c r="J5">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -740,7 +740,7 @@
         <v>0.73399999999999999</v>
       </c>
       <c r="J6">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -776,7 +776,7 @@
         <v>0.73299999999999998</v>
       </c>
       <c r="J7">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -812,7 +812,7 @@
         <v>0.73299999999999998</v>
       </c>
       <c r="J8">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -848,7 +848,7 @@
         <v>0.73099999999999998</v>
       </c>
       <c r="J9">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -884,7 +884,7 @@
         <v>0.73099999999999998</v>
       </c>
       <c r="J10">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -920,7 +920,7 @@
         <v>0.73199999999999998</v>
       </c>
       <c r="J11">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -956,7 +956,7 @@
         <v>0.73299999999999998</v>
       </c>
       <c r="J12">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -992,7 +992,7 @@
         <v>0.73499999999999999</v>
       </c>
       <c r="J13">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1028,7 +1028,7 @@
         <v>0.73699999999999999</v>
       </c>
       <c r="J14">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1064,7 +1064,7 @@
         <v>0.73899999999999999</v>
       </c>
       <c r="J15">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1100,7 +1100,7 @@
         <v>0.74199999999999999</v>
       </c>
       <c r="J16">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>